<commit_message>
organizational issues: Add TimeSchedule & Update effort-protocol
</commit_message>
<xml_diff>
--- a/Documentation/Doku_SS2017/ZeitlicherAufwand.xlsx
+++ b/Documentation/Doku_SS2017/ZeitlicherAufwand.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Quartus Prime Tutorial</t>
   </si>
@@ -104,6 +104,24 @@
   <si>
     <t>Gesamte
 Arbeitsstunden</t>
+  </si>
+  <si>
+    <t>1) Tutorial: DE0-Nano-SoC_My_First_HPS-Fpga
+2) Einrichten von Garfield Projekt in eigenes Workspace
+-&gt; Bei NIOSII Eclipse - Problem: Nicht alle Resourcen eingebunden</t>
+  </si>
+  <si>
+    <t>1) Einrichten von Garfield-Projekt
+2) Ausprobieren des NIOSII mit LED-Programm</t>
+  </si>
+  <si>
+    <t>1) Licht von Vehikel steuern
+-&gt; Codeanpassung: SetzeGPIO für Lichter angepasst</t>
+  </si>
+  <si>
+    <t>1) Erstellen Zeitplan
+2) Versuch: Compilieren von Comm_Gateway für ARM
+-&gt; Erstellen eines eigenen Makefiles =&gt; Funktioniert bisher nicht</t>
   </si>
 </sst>
 </file>
@@ -308,47 +326,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -630,10 +648,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,12 +664,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="17">
         <f>SUM(E:E)  - SUM(D:D)</f>
-        <v>0.88541666666666696</v>
+        <v>1.5902777777777786</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -695,13 +713,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="18">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="18">
+      <c r="B6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="32">
         <v>42865</v>
       </c>
       <c r="D6" s="7">
@@ -715,9 +733,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="7">
         <v>0.54166666666666663</v>
       </c>
@@ -749,13 +767,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+      <c r="A9" s="24">
         <v>4</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="30">
+      <c r="B9" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="28">
         <v>42872</v>
       </c>
       <c r="D9" s="7">
@@ -769,9 +787,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="19"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="7">
         <v>0.54166666666666663</v>
       </c>
@@ -838,7 +856,7 @@
       <c r="E13" s="13">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -849,7 +867,7 @@
       <c r="E14" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -867,21 +885,131 @@
       <c r="E15" s="13">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="13">
         <v>0.52083333333333337</v>
       </c>
       <c r="E16" s="13">
         <v>0.64583333333333337</v>
       </c>
-      <c r="F16" s="23"/>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="12">
+        <v>42893</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.46875</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="13">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="12">
+        <v>42937</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="13">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="12">
+        <v>42914</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="13">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="12">
+        <v>42947</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="A6:A7"/>

</xml_diff>

<commit_message>
Update HowTo's and current efforts
</commit_message>
<xml_diff>
--- a/Documentation/Doku_SS2017/ZeitlicherAufwand.xlsx
+++ b/Documentation/Doku_SS2017/ZeitlicherAufwand.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamMeeting" sheetId="1" r:id="rId1"/>
-    <sheet name="Baumann" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
-  <si>
-    <t>Quartus Prime Tutorial</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Datum</t>
   </si>
@@ -70,9 +66,6 @@
     <t>4) Orientierung an Projektstruktur
 -&gt; Projekt-File nicht gefunden
 -&gt; Fragen der Vorgänger-Gruppe nötig</t>
-  </si>
-  <si>
-    <t>Allein</t>
   </si>
   <si>
     <t>mit VorgängerTeam</t>
@@ -123,15 +116,345 @@
 2) Versuch: Compilieren von Comm_Gateway für ARM
 -&gt; Erstellen eines eigenen Makefiles =&gt; Funktioniert bisher nicht</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Compilieren von Comm_Gateway für ARM
+-&gt; Alle Dateien in selben Ordner =&gt; Kompilieren funktioniert mit Kommando:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>arm-linux-gnueabihf-g++ alf_data.cpp alf_data_info.cpp alf_log.cpp alf_sensors.cpp alf_sharedmemory.cpp Client_Server_impl.cpp Comm_Gateway.cpp -std=c++11 -o HSP_ARM_Gateway</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-&gt; Erstellung eines Makefiles =&gt; Funktioniert bisher nicht</t>
+    </r>
+  </si>
+  <si>
+    <t>1) Compilieren von Comm_Gateway für ARM
+-&gt; Makefile-Idee sein lassen; Nutze lieber Eclipse
+-&gt; Eclipse einrichten in Windows mit Downloads (Compiler; Make)
+     =&gt; Funktioniert noch nicht</t>
+  </si>
+  <si>
+    <t>1) Compilieren von Comm_Gateway für ARM
+-&gt; Eclipse einrichten in Windows mit Downloads (Compiler; Make)
+-&gt; Ausprobieren: Auto permanent ohne Eingabe gerade aus fahren lassen
+2) Versuch: Eclipse für Comm_Gateway-Compilierung in Repository
+-&gt; Fehlgeschlagen "src-Files, Debug-Files verschwinden nach Clean-Aufruf ?!?"
+3) Ausprobieren NIOSII-Code "Temperature als 55 anzeigen"
+-&gt; Funktioniert; aber nur temporär</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Compilieren von alf_urg.c
+-&gt; Erstellen eines eigenen Projekts in Eclipse
+-&gt; Zusätzlich: alf_urg/urg_c/src in Projekt als Include-Verzeichnis
+2) Versuch: Compilieren der GUI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Compilieren der GUI
+-&gt; Einrichten von Qt und QtCreator innerhalb der Ubuntu-VM
+nach https://wiki.ubuntuusers.de/Qt/
+-&gt; HQ von Garfield-Projekt in QtCreator ausführbar
+-&gt; Ausprobiert mit Eclipse, aber: Nicht funktioniert
+2) Auslesen von Lidar-Messwerte auf Ubuntu-VM mit Bsp-Code aus Internet
+-&gt; Lidar direkt an Rechner angeschlossen
+3) Auslesen von Lidar-Messwerte auf Garfield-Vehikel mit Main-Prg von Bsp-Code aus Internet
+= Abstandsmessung auf Garfield-Vehikel)
+4) Raussuchen von Datenblatt für Lidar-Sensor
+-&gt; Eingefügt in Git-Repo
+5) Versuch: Ausführen von Melmac_rviz auf Ubuntu-VM
+-&gt; ROS API nötig =&gt; Downloaden von http://wiki.ros.org/kinetic/Installation/Ubuntu
+</t>
+  </si>
+  <si>
+    <t>1) Problem: VM zeigt Fehler "the system is running in low-graphics mode"
+-&gt; Problem liegt am nvidia-Treiber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) BreezySlam-Alg: Betrachten der Input-Werte Timestamp, Lidar, Odometry
+-&gt; Erkenntnis: BreezySlam kann mit Lidar-Werten allein das Vehikel auf der Karte positionieren
+2) Ausführen BreezySlam auf Vehikel
+-&gt; Installieren von Make-Command war nötig
+-&gt; c++-Example auf Vehikel ausführbar
+3) Verusch: BreezySlam mit Auslesen von Lidar-Werten auf Vehikel
+-&gt; Versuch: c++-Example "log2pgm.cpp" anpassen, sodass Werte aus Lidar-Sensor genutzt werden
+=&gt;        Ausführen mit connected Lidar nicht möglich /
+oder: Nur graues Bild als Ausgabe
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  BreezySlam mit Auslesen von Lidar-Werten auf Vehikel
+-&gt; c++-Example "log2pgm.cpp" anpassen, sodass Werte aus Lidar-Sensor genutzt werden
+=&gt; Funktioniert auf VM
+=&gt; Funktioniert auf Vehikel
+=&gt; Beachte: Karte ist spiegelverkehrt
+2) Erstelle erste Version einer Karte auf Vehikel
+3) Besprechung: Ziel der Projektarbeit für Abschluss:
+-&gt; Erstellen einer lokalen Karte
+-&gt; Auslesen von Odometrie-Werte aus Rotary-Encoder für BreezySlam
+-&gt; Positionierung von Vehikel auf Karte &amp; Darstellen der Karte in GUI/HQ
+4) Einlesen von PMG-File für Verwendung in BreezySlam
+5) Versuch: Erstellen einer Karte von unserer Umgebung
+-&gt; Erstellung mit angepassten BreezySlam-Example "logmovie.py"
+-&gt; Karte nicht genau, da Odometrie-Werte fehlen
+-&gt; Bisher: Fehlgeschlagen
+</t>
+  </si>
+  <si>
+    <t>1) Versuch: Erstellen einer Karte von unserer Umgebung
+-&gt; "logmovie.py" abgeändert
+-&gt; Karte wird nach &lt;Enter&gt; erstellt
+-&gt; Karte sehr ungenau; besonders bei Drehung
+2) Email an Metzner
+3) Erweiterung von HQ-Projekt
+-&gt; Darstellen eines PGM-Files
+4) Modifizierung von BreezySlam-Example auf Vehikel
+-&gt; Vehikel misst bis Tastendruck; dannach Erzeugen eines PGM-Files</t>
+  </si>
+  <si>
+    <t>1) Finden von BreezySLAM Dokument
+2) Erweitern des HQ-Projekts
+-&gt; Punkt/Auto auf Karte anzeigen; Punkt/Auto kann sich auf Position aktualisieren
+3) Versuch: Einbinden von BreezySLAM in Garfield-ARM-Projekt
+-&gt; Eigenes Projekt zum Erzeugen der .so-SharedLibrary
+-&gt; Fehler beim Compilieren: libBreezySLAMLib.so: undefined reference to `hokuyo_connect
+-&gt; Generiertes .so-File funktioniert auf dem Vehikel im BreezySLAM-Projekt NICHT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Versuch: Compilieren von Melmac_rviz auf Ubuntu-VM
+-&gt; benötigt ROS
+-&gt; Problem beim Compilieren
+2) Einlesen in ROS Tutorial
+-&gt; Site: http://wiki.ros.org/kinetic/Installation/Ubuntu
+-&gt; nicht komplett
+3) Einarbeiten in BreezySlam
+(Site: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/simondlevy/BreezySLAM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+-&gt; Ausführen von c++-Example
+(braucht "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LIBDIR=/usr/local/lib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ldconfig</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>")
+-&gt; Ausführen von py-Example mit direkter Verbindung zu (=urgslam.py)
+   (braucht "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sudo apt-get install python-opencv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sudo apt-get install python-matplotlib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>")
+4) Einarbeiten in BreezyLidar
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://github.com/simondlevy/BreezyLidar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+-&gt; Ausführen von c++-Example
+(braucht "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chmod 777 /dev/ttyACM0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>")
+-&gt; Ausführen von python-Example
+(braucht "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sudo apt-get install python3-dev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sudo apt-get install python3-tk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>")</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Einbinden von BreezySLAM in Garfield-ARM-Projekt
+-&gt; Funktioniert; Problem war, dass .o-Files von Eclipse falsch kompiliert wurden
+2) Durchlesen von BreezySLAM-Dokumentation
+3) Versuch: Erweitere Kommunikation zw HQ und ARM sodass Position und Karte mitversendet
+4) Einbetten von BreezySLAM in Comm_Gateway Projekt
+-&gt; Hochladen von angepassten BreezySLAM-Files in Repo
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +466,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -646,12 +983,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,31 +1002,31 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="17">
         <f>SUM(E:E)  - SUM(D:D)</f>
-        <v>1.5902777777777786</v>
+        <v>4.8020833333333321</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -697,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="10">
         <v>42860</v>
@@ -709,7 +1046,7 @@
         <v>0.625</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -717,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="32">
         <v>42865</v>
@@ -729,7 +1066,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -743,7 +1080,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -751,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="11">
         <v>42866</v>
@@ -763,7 +1100,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -771,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="28">
         <v>42872</v>
@@ -783,7 +1120,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -797,7 +1134,7 @@
         <v>0.59375</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -805,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="12">
         <v>42877</v>
@@ -817,7 +1154,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -825,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="12">
         <v>42879</v>
@@ -837,7 +1174,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="87" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -845,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="12">
         <v>42884</v>
@@ -857,7 +1194,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,7 +1211,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="12">
         <v>42886</v>
@@ -886,7 +1223,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -903,7 +1240,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="12">
         <v>42893</v>
@@ -915,7 +1252,7 @@
         <v>0.46875</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -932,7 +1269,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="12">
         <v>42937</v>
@@ -944,7 +1281,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -961,7 +1298,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="12">
         <v>42914</v>
@@ -973,7 +1310,7 @@
         <v>0.5</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -985,12 +1322,12 @@
       </c>
       <c r="F22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="12">
         <v>42947</v>
@@ -1002,16 +1339,356 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="F23" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="12">
+        <v>42948</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="12">
+        <v>42949</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F25" s="22" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="26" spans="1:6" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="13">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F26" s="23"/>
+    </row>
+    <row r="27" spans="1:6" ht="45.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="12">
+        <v>42950</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="12">
+        <v>42951</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="12">
+        <v>42954</v>
+      </c>
+      <c r="D30" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="188.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="13">
+        <v>0.53125</v>
+      </c>
+      <c r="E31" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="12">
+        <v>42955</v>
+      </c>
+      <c r="D32" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E32" s="13">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="13">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E33" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" ht="105.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>19</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="12">
+        <v>42956</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="175.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E35" s="13">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>14</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="12">
+        <v>42963</v>
+      </c>
+      <c r="D36" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E36" s="13">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="E37" s="13">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:6" ht="66.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="12">
+        <v>42964</v>
+      </c>
+      <c r="D38" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E38" s="13">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="163.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="13">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E39" s="13">
+        <v>0.65625</v>
+      </c>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="12">
+        <v>42965</v>
+      </c>
+      <c r="D40" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E40" s="13">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E41" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:6" ht="64.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="12">
+        <v>42968</v>
+      </c>
+      <c r="D42" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E42" s="13">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E43" s="13">
+        <v>0.6875</v>
+      </c>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>18</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="12">
+        <v>42969</v>
+      </c>
+      <c r="D44" s="13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E44" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="13">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E45" s="13">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F45" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="21">
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F42:F43"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F32:F33"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="F13:F14"/>
@@ -1022,67 +1699,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="62" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="10">
-        <v>42864</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>